<commit_message>
complete add hero without command pattern
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtcmca-my.sharepoint.com/personal/230070312_stu_vtc_edu_hk/Documents/Sem 4/Contemporary Topics in Software Engineering/Assignment/ITP4507_Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\su\IdeaProjects\ITP4507_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{3EE924C0-90A5-4213-AFC6-79D8B0AE5A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D821847-C04B-6440-AED4-E1367C1A2252}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="2060" windowWidth="14780" windowHeight="14220" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="10290" windowHeight="13695" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>1. Create Player</t>
   </si>
@@ -106,20 +106,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -153,7 +153,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -169,9 +169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -209,7 +209,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -315,7 +315,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -457,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -468,19 +468,19 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="48.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.796875" customWidth="1"/>
-    <col min="3" max="3" width="16.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="25">
+    <row r="2" spans="1:5" ht="23.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -497,7 +497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="25">
+    <row r="3" spans="1:5" ht="23.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,18 +510,20 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="25">
+    <row r="4" spans="1:5" ht="23.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="25">
+    <row r="5" spans="1:5" ht="23.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -532,16 +534,18 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="25">
+    <row r="6" spans="1:5" ht="23.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="25">
+    <row r="7" spans="1:5" ht="23.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -554,7 +558,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="25">
+    <row r="8" spans="1:5" ht="23.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -565,7 +569,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="25">
+    <row r="9" spans="1:5" ht="23.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -576,7 +580,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="25">
+    <row r="10" spans="1:5" ht="23.25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -589,7 +593,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="25">
+    <row r="11" spans="1:5" ht="23.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -598,7 +602,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="25">
+    <row r="12" spans="1:5" ht="23.25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -607,7 +611,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="25">
+    <row r="13" spans="1:5" ht="23.25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -616,7 +620,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="25">
+    <row r="14" spans="1:5" ht="23.25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
complete function without command pattern
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\su\IdeaProjects\ITP4507_Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtcmca-my.sharepoint.com/personal/230070312_stu_vtc_edu_hk/Documents/Sem 4/Contemporary Topics in Software Engineering/Assignment/ITP4507_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3748619D-BC23-334B-B249-132439DE0525}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="10290" windowHeight="13695" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
+    <workbookView xWindow="40" yWindow="760" windowWidth="11820" windowHeight="17540" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>1. Create Player</t>
   </si>
@@ -106,20 +106,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -153,7 +153,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -169,9 +169,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主題">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -209,7 +209,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -315,7 +315,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -457,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -468,19 +468,19 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.796875" customWidth="1"/>
+    <col min="3" max="3" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="23.25">
+    <row r="2" spans="1:5" ht="25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -497,7 +497,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="23.25">
+    <row r="3" spans="1:5" ht="25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +510,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="23.25">
+    <row r="4" spans="1:5" ht="25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -523,7 +523,7 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="23.25">
+    <row r="5" spans="1:5" ht="25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -534,7 +534,7 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="23.25">
+    <row r="6" spans="1:5" ht="25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -545,7 +545,7 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="23.25">
+    <row r="7" spans="1:5" ht="25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -558,29 +558,33 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="23.25">
+    <row r="8" spans="1:5" ht="25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="23.25">
+    <row r="9" spans="1:5" ht="25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="23.25">
+    <row r="10" spans="1:5" ht="25">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -593,7 +597,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="23.25">
+    <row r="11" spans="1:5" ht="25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -602,7 +606,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="23.25">
+    <row r="12" spans="1:5" ht="25">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -611,7 +615,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="23.25">
+    <row r="13" spans="1:5" ht="25">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -620,7 +624,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="23.25">
+    <row r="14" spans="1:5" ht="25">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
complete command pattern without undo/redo
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtcmca-my.sharepoint.com/personal/230070312_stu_vtc_edu_hk/Documents/Sem 4/Contemporary Topics in Software Engineering/Assignment/ITP4507_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75F1E7CC-69A1-8C48-970A-E5AA1F6CB780}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB402F06-9BB0-814B-87F6-F83E9E235B86}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="760" windowWidth="27160" windowHeight="17780" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>1. Create Player</t>
   </si>
@@ -468,7 +468,7 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -522,7 +522,9 @@
       <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="25">
@@ -576,7 +578,9 @@
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="25">
@@ -602,7 +606,9 @@
       <c r="C10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" ht="25">

</xml_diff>

<commit_message>
complete all command pattern without undo/redo
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtcmca-my.sharepoint.com/personal/230070312_stu_vtc_edu_hk/Documents/Sem 4/Contemporary Topics in Software Engineering/Assignment/ITP4507_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB402F06-9BB0-814B-87F6-F83E9E235B86}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE0D6E0F-4045-364B-A25B-C7C7EC3AE698}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="760" windowWidth="27160" windowHeight="17780" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>1. Create Player</t>
   </si>
@@ -102,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +121,15 @@
       <sz val="9"/>
       <name val="新細明體"/>
       <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -145,11 +154,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -468,32 +481,32 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="48.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.796875" customWidth="1"/>
+    <col min="2" max="2" width="57" customWidth="1"/>
     <col min="3" max="3" width="16.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -593,7 +606,9 @@
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="25">
@@ -617,7 +632,9 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="25">

</xml_diff>

<commit_message>
complete createPlayerCommandFactory with undo/redo
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtcmca-my.sharepoint.com/personal/230070312_stu_vtc_edu_hk/Documents/Sem 4/Contemporary Topics in Software Engineering/Assignment/ITP4507_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DE0D6E0F-4045-364B-A25B-C7C7EC3AE698}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAE50279-244D-8A45-A6DE-C2C3E6C2F2DF}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="760" windowWidth="27160" windowHeight="17780" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
   <si>
     <t>1. Create Player</t>
   </si>
@@ -95,6 +95,10 @@
   </si>
   <si>
     <t>Implement without command pattern</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y (OK)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -481,13 +485,13 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="48.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57" customWidth="1"/>
+    <col min="2" max="2" width="57" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="16.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.19921875" bestFit="1" customWidth="1"/>
@@ -518,12 +522,14 @@
         <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="25">
       <c r="A4" s="1" t="s">
@@ -643,7 +649,9 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" ht="25">
@@ -652,7 +660,9 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" ht="25">

</xml_diff>

<commit_message>
update comment to indicate no implementation on undo/redo
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtcmca-my.sharepoint.com/personal/230070312_stu_vtc_edu_hk/Documents/Sem 4/Contemporary Topics in Software Engineering/Assignment/ITP4507_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAE50279-244D-8A45-A6DE-C2C3E6C2F2DF}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9584F3A0-45FE-DC48-B59B-70FE4FBAABD7}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="760" windowWidth="27160" windowHeight="17780" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17400" windowHeight="17780" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>1. Create Player</t>
   </si>
@@ -485,14 +485,14 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="48.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="57" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.19921875" bestFit="1" customWidth="1"/>
   </cols>
@@ -579,9 +579,7 @@
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
command factory of no need undo/redo command
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtcmca-my.sharepoint.com/personal/230070312_stu_vtc_edu_hk/Documents/Sem 4/Contemporary Topics in Software Engineering/Assignment/ITP4507_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9584F3A0-45FE-DC48-B59B-70FE4FBAABD7}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FBF2D65-56B2-754D-8FE0-27EF69A3DD4E}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="17400" windowHeight="17780" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>1. Create Player</t>
   </si>
@@ -485,7 +485,7 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -557,7 +557,9 @@
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="25">
       <c r="A6" s="1" t="s">
@@ -570,7 +572,9 @@
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="25">
       <c r="A7" s="1" t="s">
@@ -583,7 +587,9 @@
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="25">
       <c r="A8" s="1" t="s">
@@ -639,7 +645,9 @@
       <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="25">
       <c r="A12" s="1" t="s">
@@ -650,7 +658,9 @@
       <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="25">
       <c r="A13" s="1" t="s">
@@ -661,7 +671,9 @@
       <c r="D13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="25">
       <c r="A14" s="1" t="s">
@@ -674,7 +686,9 @@
       <c r="D14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
command factory (except call hero skill and change player name)
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtcmca-my.sharepoint.com/personal/230070312_stu_vtc_edu_hk/Documents/Sem 4/Contemporary Topics in Software Engineering/Assignment/ITP4507_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FBF2D65-56B2-754D-8FE0-27EF69A3DD4E}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{844853EF-7498-7543-830C-D66E7BDE27DC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17400" windowHeight="17780" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="10120" windowHeight="17780" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="21">
   <si>
     <t>1. Create Player</t>
   </si>
@@ -138,12 +138,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -158,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -168,6 +174,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -183,6 +190,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -485,7 +496,8 @@
   <dimension ref="A2:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -539,12 +551,14 @@
         <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="25">
       <c r="A5" s="1" t="s">
@@ -592,7 +606,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -619,10 +633,12 @@
       <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">

</xml_diff>

<commit_message>
create basic structure of memento
</commit_message>
<xml_diff>
--- a/checklist.xlsx
+++ b/checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vtcmca-my.sharepoint.com/personal/230070312_stu_vtc_edu_hk/Documents/Sem 4/Contemporary Topics in Software Engineering/Assignment/ITP4507_Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{844853EF-7498-7543-830C-D66E7BDE27DC}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="13_ncr:1_{E638D71A-1F0C-4144-AC59-29F6CD2605A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51EB78D3-FA72-7841-A469-7F2EBA253EDF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="10120" windowHeight="17780" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="14000" windowHeight="17780" xr2:uid="{1491E1C1-050E-49D3-8E13-06AAE90AAF13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -497,7 +497,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C9" sqref="C9"/>
+      <selection pane="topRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -628,7 +628,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>18</v>

</xml_diff>